<commit_message>
start of auto-gen insilico lod text
</commit_message>
<xml_diff>
--- a/explore/openCyto/p1Checks/extraMiss.xlsx
+++ b/explore/openCyto/p1Checks/extraMiss.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kitty/git/auto-fcs/explore/openCyto/p1Checks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9020CE57-305F-A84D-8355-47E20A48BE41}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369CEA39-A313-584C-8059-BE00DEDB0C02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="460" windowWidth="26720" windowHeight="15540" xr2:uid="{556BC6EB-8FDB-424F-8DBC-0D2721456954}"/>
+    <workbookView xWindow="15320" yWindow="1480" windowWidth="26720" windowHeight="15540" xr2:uid="{556BC6EB-8FDB-424F-8DBC-0D2721456954}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -727,7 +727,7 @@
   <dimension ref="A1:E107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A1:B28"/>
+      <selection activeCell="A19" sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -740,7 +740,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="str">
-        <f>VLOOKUP(A1,E:E,1,FALSE)</f>
+        <f t="shared" ref="B1:B28" si="0">VLOOKUP(A1,E:E,1,FALSE)</f>
         <v>2016-12-05_PANEL 1_DHS_Group one_F1652314_002.fcs</v>
       </c>
       <c r="E1" t="s">
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f>VLOOKUP(A2,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2016-12-22_PANEL 1_HB_group one_F1635968_016.fcs</v>
       </c>
       <c r="E2" t="s">
@@ -764,7 +764,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="str">
-        <f>VLOOKUP(A3,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-04-11_PANEL 1_LSR_RR_Group one_F1642913_005.fcs</v>
       </c>
       <c r="E3" t="s">
@@ -776,7 +776,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="str">
-        <f>VLOOKUP(A4,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-04-11_PANEL 1_LSR_RR_Group two_F1642674_038.fcs</v>
       </c>
       <c r="E4" t="s">
@@ -788,7 +788,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="str">
-        <f>VLOOKUP(A5,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-04-21_PANEL 1_LSR_ZF_Group one_F1642945_002.fcs</v>
       </c>
       <c r="E5" t="s">
@@ -800,7 +800,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="str">
-        <f>VLOOKUP(A6,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-05-01_PANEL 1_FORTESSA_DHS_group one_F1640773_019.fcs</v>
       </c>
       <c r="E6" t="s">
@@ -812,7 +812,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="str">
-        <f>VLOOKUP(A7,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-05-18_PANEL 1_FORTESSA_ZF_HB_group one_HB_F1635108_030.fcs</v>
       </c>
       <c r="E7" t="s">
@@ -824,7 +824,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="str">
-        <f>VLOOKUP(A8,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-06-20_PANEL 1_FORTESSA_DHS_group one_RR_F1632752_035.fcs</v>
       </c>
       <c r="E8" t="s">
@@ -836,7 +836,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="str">
-        <f>VLOOKUP(A9,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-07-07_PANEL 1_FORTESSA_ZF_group two_ZF_F1640046_019.fcs</v>
       </c>
       <c r="E9" t="s">
@@ -848,7 +848,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="str">
-        <f>VLOOKUP(A10,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_FORTESSA_DHS_group two_DHS_F1632601_021.fcs</v>
       </c>
       <c r="E10" t="s">
@@ -860,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="str">
-        <f>VLOOKUP(A11,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_FORTESSA_DHS_group two_DHS_F1633089_019.fcs</v>
       </c>
       <c r="E11" t="s">
@@ -872,7 +872,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="str">
-        <f>VLOOKUP(A12,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_FORTESSA_DHS_group two_DHS_F1642244_023.fcs</v>
       </c>
       <c r="E12" t="s">
@@ -884,7 +884,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="str">
-        <f>VLOOKUP(A13,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_FORTESSA_DHS_group two_DHS_F1642289_020.fcs</v>
       </c>
       <c r="E13" t="s">
@@ -896,7 +896,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="str">
-        <f>VLOOKUP(A14,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_FORTESSA_DHS_group two_DHS_F1642512_022.fcs</v>
       </c>
       <c r="E14" t="s">
@@ -908,7 +908,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="str">
-        <f>VLOOKUP(A15,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_LSR_DHS_Group two_DHS_F1637738_020.fcs</v>
       </c>
       <c r="E15" t="s">
@@ -920,7 +920,7 @@
         <v>24</v>
       </c>
       <c r="B16" t="str">
-        <f>VLOOKUP(A16,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_LSR_DHS_Group two_DHS_F1642242_021.fcs</v>
       </c>
       <c r="E16" t="s">
@@ -932,7 +932,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="str">
-        <f>VLOOKUP(A17,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_LSR_DHS_Group two_DHS_F1642243_023.fcs</v>
       </c>
       <c r="E17" t="s">
@@ -944,7 +944,7 @@
         <v>26</v>
       </c>
       <c r="B18" t="str">
-        <f>VLOOKUP(A18,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_LSR_DHS_Group two_DHS_F1642462_019.fcs</v>
       </c>
       <c r="E18" t="s">
@@ -956,7 +956,7 @@
         <v>30</v>
       </c>
       <c r="B19" t="str">
-        <f>VLOOKUP(A19,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>2017-08-08_PANEL 1_LSR_DHS_Group two_DHS_F1642516_022.fcs</v>
       </c>
       <c r="E19" t="s">
@@ -968,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="e">
-        <f>VLOOKUP(A20,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E20" t="s">
@@ -980,7 +980,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="e">
-        <f>VLOOKUP(A21,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E21" t="s">
@@ -992,7 +992,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="e">
-        <f>VLOOKUP(A22,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E22" t="s">
@@ -1004,7 +1004,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="e">
-        <f>VLOOKUP(A23,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E23" t="s">
@@ -1016,7 +1016,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="e">
-        <f>VLOOKUP(A24,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E24" t="s">
@@ -1028,7 +1028,7 @@
         <v>7</v>
       </c>
       <c r="B25" t="e">
-        <f>VLOOKUP(A25,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E25" t="s">
@@ -1040,7 +1040,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="e">
-        <f>VLOOKUP(A26,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E26" t="s">
@@ -1052,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="B27" t="e">
-        <f>VLOOKUP(A27,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E27" t="s">
@@ -1064,7 +1064,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="e">
-        <f>VLOOKUP(A28,E:E,1,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
       <c r="E28" t="s">

</xml_diff>